<commit_message>
Completed Compositions for Diagnostic FHIR IG
Closes #33 and Closes #41
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/composition-imagreport-1.xlsx
+++ b/output/DiagnosticReport/composition-imagreport-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2529" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2528" uniqueCount="473">
   <si>
     <t>Path</t>
   </si>
@@ -159,7 +159,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}inv-dh-cmp-01:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt; 1).exists()}inv-dh-cmp-02:The author shall at least have a reference or an identifier with at least a system and a value {author.reference.exists() or author.identifier.where(system.count() + value.count() &gt; 1).exists()}inv-dh-cmp-03:The custodian shall at least have a reference or an identifier with at least a system and a value {custodian.reference.exists() or custodian.identifier.where(system.count() + value.count() &gt; 1).exists()}</t>
   </si>
   <si>
     <t>Event</t>
@@ -215,81 +215,85 @@
     <t>Resource.meta</t>
   </si>
   <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+inv-dh-cmp-04:One profile shall be 'http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/composition-imagreport-1' {profile.where($this='http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/composition-imagreport-1').exists()}</t>
+  </si>
+  <si>
+    <t>Composition.meta.id</t>
+  </si>
+  <si>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Composition.meta.extension</t>
+  </si>
+  <si>
+    <t>extensions
+user content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension
+</t>
+  </si>
+  <si>
+    <t>Additional content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+  </si>
+  <si>
+    <t>Composition.meta.versionId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id
+</t>
+  </si>
+  <si>
+    <t>Version specific identifier</t>
+  </si>
+  <si>
+    <t>The version specific identifier, as it appears in the version portion of the URL. This value changes when the resource is created, updated, or deleted.</t>
+  </si>
+  <si>
+    <t>The server assigns this value, and ignores what the client specifies, except in the case that the server is imposing version integrity on updates/deletes.</t>
+  </si>
+  <si>
+    <t>Meta.versionId</t>
+  </si>
+  <si>
     <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 </t>
   </si>
   <si>
-    <t>Composition.meta.id</t>
-  </si>
-  <si>
-    <t>Unique id for inter-element referencing</t>
-  </si>
-  <si>
-    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
-  </si>
-  <si>
-    <t>Element.id</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
-    <t>Composition.meta.extension</t>
-  </si>
-  <si>
-    <t>extensions
-user content</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension
-</t>
-  </si>
-  <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:url}
-</t>
-  </si>
-  <si>
-    <t>Extensions are always sliced by (at least) url</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>Element.extension</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
-  </si>
-  <si>
-    <t>Composition.meta.versionId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id
-</t>
-  </si>
-  <si>
-    <t>Version specific identifier</t>
-  </si>
-  <si>
-    <t>The version specific identifier, as it appears in the version portion of the URL. This value changes when the resource is created, updated, or deleted.</t>
-  </si>
-  <si>
-    <t>The server assigns this value, and ignores what the client specifies, except in the case that the server is imposing version integrity on updates/deletes.</t>
-  </si>
-  <si>
-    <t>Meta.versionId</t>
-  </si>
-  <si>
     <t>Composition.meta.lastUpdated</t>
   </si>
   <si>
@@ -577,7 +581,7 @@
     <t>Composition.status</t>
   </si>
   <si>
-    <t>preliminary | final | amended | entered-in-error</t>
+    <t>preliminary | final | amended</t>
   </si>
   <si>
     <t>The workflow/clinical status of this composition. The status is a marker for the clinical standing of the document.</t>
@@ -593,10 +597,7 @@
     <t>required</t>
   </si>
   <si>
-    <t>The workflow/clinical status of the composition.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/composition-status|4.0.1</t>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/compositionstatus-document-available-1</t>
   </si>
   <si>
     <t>Event.status</t>
@@ -692,7 +693,7 @@
     <t>Composition.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/patient-mhr-1|http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/patient-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/patient-mhr-1|http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/patient-ident-1)
 </t>
   </si>
   <si>
@@ -788,7 +789,7 @@
     <t>Composition.author</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/practitionerrole-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/practitionerrole-ident-1)
 </t>
   </si>
   <si>
@@ -880,6 +881,10 @@
     <t>Identifies responsibility for the accuracy of the composition content.</t>
   </si>
   <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+inv-dh-cmp-05:The party shall at least have a reference or an identifier with at least a system and a value {party.reference.exists() or party.identifier.where(system.count() + value.count() &gt; 1).exists()}</t>
+  </si>
+  <si>
     <t>.participation[typeCode="AUTHEN"].role[classCode="ASSIGNED"]</t>
   </si>
   <si>
@@ -981,7 +986,7 @@
     <t>Composition.custodian</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/organization-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/organization-ident-1)
 </t>
   </si>
   <si>
@@ -1670,7 +1675,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="95.7734375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="73.27734375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="82.76171875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
@@ -2472,7 +2477,7 @@
         <v>41</v>
       </c>
       <c r="AI7" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ7" t="s" s="2">
         <v>41</v>
@@ -2492,7 +2497,7 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
@@ -2515,16 +2520,16 @@
         <v>54</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
@@ -2574,7 +2579,7 @@
         <v>41</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>42</v>
@@ -2586,7 +2591,7 @@
         <v>41</v>
       </c>
       <c r="AI8" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ8" t="s" s="2">
         <v>41</v>
@@ -2606,7 +2611,7 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
@@ -2629,16 +2634,16 @@
         <v>54</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
@@ -2688,7 +2693,7 @@
         <v>41</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>42</v>
@@ -2700,7 +2705,7 @@
         <v>41</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ9" t="s" s="2">
         <v>41</v>
@@ -2720,7 +2725,7 @@
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
@@ -2743,16 +2748,16 @@
         <v>54</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
@@ -2802,7 +2807,7 @@
         <v>41</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>42</v>
@@ -2814,7 +2819,7 @@
         <v>41</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ10" t="s" s="2">
         <v>41</v>
@@ -2834,7 +2839,7 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
@@ -2857,16 +2862,16 @@
         <v>54</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" t="s" s="2">
@@ -2892,13 +2897,13 @@
         <v>41</v>
       </c>
       <c r="W11" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="X11" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Y11" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Z11" t="s" s="2">
         <v>41</v>
@@ -2916,7 +2921,7 @@
         <v>41</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>42</v>
@@ -2928,7 +2933,7 @@
         <v>41</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ11" t="s" s="2">
         <v>41</v>
@@ -2948,7 +2953,7 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -2971,16 +2976,16 @@
         <v>54</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
@@ -3006,13 +3011,13 @@
         <v>41</v>
       </c>
       <c r="W12" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="X12" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="Y12" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="Z12" t="s" s="2">
         <v>41</v>
@@ -3030,7 +3035,7 @@
         <v>41</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>42</v>
@@ -3042,7 +3047,7 @@
         <v>41</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ12" t="s" s="2">
         <v>41</v>
@@ -3062,7 +3067,7 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -3085,16 +3090,16 @@
         <v>54</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
@@ -3144,7 +3149,7 @@
         <v>41</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>42</v>
@@ -3156,7 +3161,7 @@
         <v>41</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ13" t="s" s="2">
         <v>41</v>
@@ -3176,7 +3181,7 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -3199,16 +3204,16 @@
         <v>41</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
@@ -3216,7 +3221,7 @@
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="R14" t="s" s="2">
         <v>41</v>
@@ -3234,13 +3239,13 @@
         <v>41</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>41</v>
@@ -3258,7 +3263,7 @@
         <v>41</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>42</v>
@@ -3270,7 +3275,7 @@
         <v>41</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ14" t="s" s="2">
         <v>41</v>
@@ -3290,11 +3295,11 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
@@ -3313,16 +3318,16 @@
         <v>41</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
@@ -3372,7 +3377,7 @@
         <v>41</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>42</v>
@@ -3384,13 +3389,13 @@
         <v>41</v>
       </c>
       <c r="AI15" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ15" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AL15" t="s" s="2">
         <v>41</v>
@@ -3404,11 +3409,11 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
@@ -3427,16 +3432,16 @@
         <v>41</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
@@ -3486,7 +3491,7 @@
         <v>41</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>42</v>
@@ -3504,7 +3509,7 @@
         <v>41</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AL16" t="s" s="2">
         <v>41</v>
@@ -3518,7 +3523,7 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3544,10 +3549,10 @@
         <v>73</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -3596,7 +3601,7 @@
         <v>79</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>42</v>
@@ -3628,10 +3633,10 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C18" t="s" s="2">
         <v>41</v>
@@ -3653,13 +3658,13 @@
         <v>41</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -3710,7 +3715,7 @@
         <v>41</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>42</v>
@@ -3719,7 +3724,7 @@
         <v>43</v>
       </c>
       <c r="AH18" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AI18" t="s" s="2">
         <v>81</v>
@@ -3742,7 +3747,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3768,16 +3773,16 @@
         <v>73</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="M19" t="s" s="2">
         <v>76</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="O19" t="s" s="2">
         <v>41</v>
@@ -3826,7 +3831,7 @@
         <v>41</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>42</v>
@@ -3844,7 +3849,7 @@
         <v>41</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>41</v>
@@ -3858,7 +3863,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3881,16 +3886,16 @@
         <v>54</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
@@ -3940,7 +3945,7 @@
         <v>41</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>42</v>
@@ -3952,27 +3957,27 @@
         <v>41</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3995,19 +4000,19 @@
         <v>54</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>41</v>
@@ -4032,11 +4037,9 @@
         <v>41</v>
       </c>
       <c r="W21" t="s" s="2">
-        <v>183</v>
-      </c>
-      <c r="X21" t="s" s="2">
         <v>184</v>
       </c>
+      <c r="X21" s="2"/>
       <c r="Y21" t="s" s="2">
         <v>185</v>
       </c>
@@ -4056,7 +4059,7 @@
         <v>41</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>53</v>
@@ -4068,7 +4071,7 @@
         <v>41</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ21" t="s" s="2">
         <v>186</v>
@@ -4148,7 +4151,7 @@
         <v>41</v>
       </c>
       <c r="W22" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="X22" t="s" s="2">
         <v>197</v>
@@ -4184,7 +4187,7 @@
         <v>41</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ22" t="s" s="2">
         <v>199</v>
@@ -4264,7 +4267,7 @@
         <v>41</v>
       </c>
       <c r="W23" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="X23" t="s" s="2">
         <v>209</v>
@@ -4300,7 +4303,7 @@
         <v>41</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ23" t="s" s="2">
         <v>211</v>
@@ -4416,7 +4419,7 @@
         <v>41</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ24" t="s" s="2">
         <v>41</v>
@@ -4530,7 +4533,7 @@
         <v>41</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ25" t="s" s="2">
         <v>229</v>
@@ -4646,7 +4649,7 @@
         <v>41</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ26" t="s" s="2">
         <v>240</v>
@@ -4760,7 +4763,7 @@
         <v>41</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ27" t="s" s="2">
         <v>250</v>
@@ -4874,7 +4877,7 @@
         <v>41</v>
       </c>
       <c r="AI28" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ28" t="s" s="2">
         <v>41</v>
@@ -4917,7 +4920,7 @@
         <v>54</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K29" t="s" s="2">
         <v>263</v>
@@ -4952,7 +4955,7 @@
         <v>41</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="X29" t="s" s="2">
         <v>266</v>
@@ -4988,7 +4991,7 @@
         <v>41</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ29" t="s" s="2">
         <v>41</v>
@@ -5104,19 +5107,19 @@
         <v>41</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>65</v>
+        <v>276</v>
       </c>
       <c r="AJ30" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>41</v>
@@ -5124,7 +5127,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5236,7 +5239,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5350,11 +5353,11 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
@@ -5376,16 +5379,16 @@
         <v>73</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M33" t="s" s="2">
         <v>76</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>41</v>
@@ -5434,7 +5437,7 @@
         <v>41</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>42</v>
@@ -5452,7 +5455,7 @@
         <v>41</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AL33" t="s" s="2">
         <v>41</v>
@@ -5466,7 +5469,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5489,24 +5492,24 @@
         <v>41</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="O34" t="s" s="2">
         <v>41</v>
       </c>
       <c r="P34" s="2"/>
       <c r="Q34" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="R34" t="s" s="2">
         <v>41</v>
@@ -5524,13 +5527,13 @@
         <v>41</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="X34" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>41</v>
@@ -5548,7 +5551,7 @@
         <v>41</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>53</v>
@@ -5560,16 +5563,16 @@
         <v>41</v>
       </c>
       <c r="AI34" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ34" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AM34" t="s" s="2">
         <v>41</v>
@@ -5580,7 +5583,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5606,14 +5609,14 @@
         <v>235</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="O35" t="s" s="2">
         <v>41</v>
@@ -5662,7 +5665,7 @@
         <v>41</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>42</v>
@@ -5674,16 +5677,16 @@
         <v>41</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ35" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AM35" t="s" s="2">
         <v>41</v>
@@ -5694,7 +5697,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5720,14 +5723,14 @@
         <v>246</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="O36" t="s" s="2">
         <v>41</v>
@@ -5776,7 +5779,7 @@
         <v>41</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>42</v>
@@ -5788,27 +5791,27 @@
         <v>41</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ36" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AM36" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5831,19 +5834,19 @@
         <v>54</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>41</v>
@@ -5892,7 +5895,7 @@
         <v>41</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>42</v>
@@ -5904,19 +5907,19 @@
         <v>41</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>41</v>
@@ -5924,7 +5927,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5950,13 +5953,13 @@
         <v>271</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
@@ -6006,7 +6009,7 @@
         <v>41</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>42</v>
@@ -6018,19 +6021,19 @@
         <v>41</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ38" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>41</v>
@@ -6038,7 +6041,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6150,7 +6153,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6264,11 +6267,11 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
@@ -6290,16 +6293,16 @@
         <v>73</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M41" t="s" s="2">
         <v>76</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>41</v>
@@ -6348,7 +6351,7 @@
         <v>41</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>42</v>
@@ -6366,7 +6369,7 @@
         <v>41</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>41</v>
@@ -6380,7 +6383,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6403,16 +6406,16 @@
         <v>41</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6438,13 +6441,13 @@
         <v>41</v>
       </c>
       <c r="W42" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="Y42" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="Z42" t="s" s="2">
         <v>41</v>
@@ -6462,7 +6465,7 @@
         <v>41</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>53</v>
@@ -6474,19 +6477,19 @@
         <v>41</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ42" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>41</v>
@@ -6494,7 +6497,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6517,13 +6520,13 @@
         <v>41</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -6574,7 +6577,7 @@
         <v>41</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>53</v>
@@ -6586,19 +6589,19 @@
         <v>41</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ43" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>41</v>
@@ -6606,7 +6609,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6632,16 +6635,16 @@
         <v>271</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="O44" t="s" s="2">
         <v>41</v>
@@ -6690,7 +6693,7 @@
         <v>41</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>42</v>
@@ -6702,19 +6705,19 @@
         <v>41</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ44" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>41</v>
@@ -6722,7 +6725,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6834,7 +6837,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6948,11 +6951,11 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
@@ -6974,16 +6977,16 @@
         <v>73</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M47" t="s" s="2">
         <v>76</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>41</v>
@@ -7032,7 +7035,7 @@
         <v>41</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>42</v>
@@ -7050,7 +7053,7 @@
         <v>41</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>41</v>
@@ -7064,7 +7067,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7090,13 +7093,13 @@
         <v>191</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
@@ -7122,13 +7125,13 @@
         <v>41</v>
       </c>
       <c r="W48" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>41</v>
@@ -7146,7 +7149,7 @@
         <v>41</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>42</v>
@@ -7158,7 +7161,7 @@
         <v>41</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ48" t="s" s="2">
         <v>41</v>
@@ -7170,7 +7173,7 @@
         <v>201</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>41</v>
@@ -7178,7 +7181,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7201,13 +7204,13 @@
         <v>54</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -7258,7 +7261,7 @@
         <v>41</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>42</v>
@@ -7270,7 +7273,7 @@
         <v>41</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ49" t="s" s="2">
         <v>41</v>
@@ -7282,7 +7285,7 @@
         <v>242</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>41</v>
@@ -7290,7 +7293,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7313,13 +7316,13 @@
         <v>54</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -7370,7 +7373,7 @@
         <v>41</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>42</v>
@@ -7382,13 +7385,13 @@
         <v>41</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ50" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>70</v>
@@ -7402,7 +7405,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7428,10 +7431,10 @@
         <v>271</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -7482,7 +7485,7 @@
         <v>41</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>42</v>
@@ -7494,16 +7497,16 @@
         <v>41</v>
       </c>
       <c r="AI51" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AJ51" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AM51" t="s" s="2">
         <v>41</v>
@@ -7514,7 +7517,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7626,7 +7629,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7740,11 +7743,11 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" t="s" s="2">
@@ -7766,16 +7769,16 @@
         <v>73</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M54" t="s" s="2">
         <v>76</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>41</v>
@@ -7824,7 +7827,7 @@
         <v>41</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>42</v>
@@ -7842,7 +7845,7 @@
         <v>41</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AL54" t="s" s="2">
         <v>41</v>
@@ -7856,11 +7859,11 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
@@ -7882,16 +7885,16 @@
         <v>55</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="N55" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>41</v>
@@ -7940,7 +7943,7 @@
         <v>41</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>42</v>
@@ -7952,7 +7955,7 @@
         <v>41</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ55" t="s" s="2">
         <v>41</v>
@@ -7972,7 +7975,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7998,16 +8001,16 @@
         <v>191</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="N56" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>41</v>
@@ -8017,7 +8020,7 @@
         <v>41</v>
       </c>
       <c r="R56" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="S56" t="s" s="2">
         <v>41</v>
@@ -8032,13 +8035,13 @@
         <v>41</v>
       </c>
       <c r="W56" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="X56" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="Y56" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="Z56" t="s" s="2">
         <v>41</v>
@@ -8056,7 +8059,7 @@
         <v>41</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>42</v>
@@ -8068,7 +8071,7 @@
         <v>41</v>
       </c>
       <c r="AI56" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ56" t="s" s="2">
         <v>41</v>
@@ -8088,7 +8091,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -8111,13 +8114,13 @@
         <v>41</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M57" s="2"/>
       <c r="N57" t="s" s="2">
@@ -8170,7 +8173,7 @@
         <v>41</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>42</v>
@@ -8182,7 +8185,7 @@
         <v>41</v>
       </c>
       <c r="AI57" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ57" t="s" s="2">
         <v>41</v>
@@ -8202,7 +8205,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -8225,16 +8228,16 @@
         <v>41</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" t="s" s="2">
@@ -8284,7 +8287,7 @@
         <v>41</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>42</v>
@@ -8296,7 +8299,7 @@
         <v>41</v>
       </c>
       <c r="AI58" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ58" t="s" s="2">
         <v>41</v>
@@ -8305,7 +8308,7 @@
         <v>41</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="AM58" t="s" s="2">
         <v>41</v>
@@ -8316,7 +8319,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8339,16 +8342,16 @@
         <v>41</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
@@ -8398,7 +8401,7 @@
         <v>41</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>42</v>
@@ -8407,19 +8410,19 @@
         <v>53</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AI59" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ59" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="AM59" t="s" s="2">
         <v>41</v>
@@ -8430,7 +8433,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8453,26 +8456,26 @@
         <v>41</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>41</v>
       </c>
       <c r="P60" s="2"/>
       <c r="Q60" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="R60" t="s" s="2">
         <v>41</v>
@@ -8490,13 +8493,13 @@
         <v>41</v>
       </c>
       <c r="W60" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="X60" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="Y60" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="Z60" t="s" s="2">
         <v>41</v>
@@ -8514,7 +8517,7 @@
         <v>41</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>42</v>
@@ -8526,13 +8529,13 @@
         <v>41</v>
       </c>
       <c r="AI60" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ60" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>70</v>
@@ -8546,7 +8549,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8572,16 +8575,16 @@
         <v>191</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="N61" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>41</v>
@@ -8606,13 +8609,13 @@
         <v>41</v>
       </c>
       <c r="W61" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="Z61" t="s" s="2">
         <v>41</v>
@@ -8630,7 +8633,7 @@
         <v>41</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>42</v>
@@ -8642,13 +8645,13 @@
         <v>41</v>
       </c>
       <c r="AI61" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ61" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="AL61" t="s" s="2">
         <v>70</v>
@@ -8662,7 +8665,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8685,16 +8688,16 @@
         <v>41</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="K62" t="s" s="2">
         <v>44</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
@@ -8744,7 +8747,7 @@
         <v>41</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>42</v>
@@ -8753,19 +8756,19 @@
         <v>43</v>
       </c>
       <c r="AH62" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="AI62" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ62" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AM62" t="s" s="2">
         <v>41</v>
@@ -8776,7 +8779,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8888,7 +8891,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -9002,7 +9005,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -9028,13 +9031,13 @@
         <v>55</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="N65" s="2"/>
       <c r="O65" t="s" s="2">
@@ -9084,7 +9087,7 @@
         <v>41</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>42</v>
@@ -9093,16 +9096,16 @@
         <v>53</v>
       </c>
       <c r="AH65" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="AI65" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ65" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>41</v>
@@ -9116,7 +9119,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -9139,16 +9142,16 @@
         <v>54</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
@@ -9174,13 +9177,13 @@
         <v>41</v>
       </c>
       <c r="W66" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="X66" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="Y66" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="Z66" t="s" s="2">
         <v>41</v>
@@ -9198,7 +9201,7 @@
         <v>41</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>42</v>
@@ -9210,13 +9213,13 @@
         <v>41</v>
       </c>
       <c r="AI66" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ66" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AL66" t="s" s="2">
         <v>41</v>
@@ -9230,7 +9233,7 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -9253,16 +9256,16 @@
         <v>54</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="N67" s="2"/>
       <c r="O67" t="s" s="2">
@@ -9312,7 +9315,7 @@
         <v>41</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>42</v>
@@ -9324,13 +9327,13 @@
         <v>41</v>
       </c>
       <c r="AI67" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ67" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AL67" t="s" s="2">
         <v>41</v>
@@ -9344,7 +9347,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -9370,13 +9373,13 @@
         <v>55</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="N68" s="2"/>
       <c r="O68" t="s" s="2">
@@ -9426,7 +9429,7 @@
         <v>41</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>42</v>
@@ -9438,13 +9441,13 @@
         <v>41</v>
       </c>
       <c r="AI68" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ68" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK68" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AL68" t="s" s="2">
         <v>41</v>
@@ -9458,7 +9461,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -9484,16 +9487,16 @@
         <v>191</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="M69" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="N69" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="O69" t="s" s="2">
         <v>41</v>
@@ -9518,13 +9521,13 @@
         <v>41</v>
       </c>
       <c r="W69" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="X69" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="Y69" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="Z69" t="s" s="2">
         <v>41</v>
@@ -9542,7 +9545,7 @@
         <v>41</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>42</v>
@@ -9551,16 +9554,16 @@
         <v>53</v>
       </c>
       <c r="AH69" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="AI69" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ69" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK69" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="AL69" t="s" s="2">
         <v>70</v>
@@ -9574,7 +9577,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -9600,13 +9603,13 @@
         <v>41</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="N70" s="2"/>
       <c r="O70" t="s" s="2">
@@ -9656,7 +9659,7 @@
         <v>41</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>42</v>
@@ -9665,19 +9668,19 @@
         <v>43</v>
       </c>
       <c r="AH70" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AI70" t="s" s="2">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="AJ70" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AK70" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AL70" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="AM70" t="s" s="2">
         <v>41</v>

</xml_diff>